<commit_message>
Update keywords.xlsx - Add/modify keywords for better matching
</commit_message>
<xml_diff>
--- a/keywords.xlsx
+++ b/keywords.xlsx
@@ -1,20 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wepapp\brand-matching2\newmatch\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB9A9E16-3443-43BC-9BB3-989EF212DBAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="21300" yWindow="2970" windowWidth="23700" windowHeight="16545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>키워드</t>
   </si>
@@ -124,9 +143,6 @@
     <t>*</t>
   </si>
   <si>
-    <t>~</t>
-  </si>
-  <si>
     <t>*XL*</t>
   </si>
   <si>
@@ -134,17 +150,45 @@
   </si>
   <si>
     <t>*M~L*</t>
+  </si>
+  <si>
+    <t>(XXL~JL)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>(25겨울)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>(13~19)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>(XXL~3XL)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>(S~XXL)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>(7~11)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>(17~19)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -152,8 +196,15 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -199,17 +250,25 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -247,7 +306,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -281,6 +340,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -315,9 +375,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -490,214 +551,247 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:A46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
-      <c r="A38" t="s">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
-      <c r="A39" t="s">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
-      <c r="A40" t="s">
-        <v>39</v>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>